<commit_message>
add oww2 base, addons, rci, and bdk packages
</commit_message>
<xml_diff>
--- a/src/yaml/stex-custodian/CDK3 Progress.xlsx
+++ b/src/yaml/stex-custodian/CDK3 Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\repos\simtropolis-channel\src\yaml\stex-custodian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6963D7AC-BAEE-4A73-A3EC-6660AB801DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438E5D5F-0476-4653-8B63-4201910ECE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2376" yWindow="17172" windowWidth="34776" windowHeight="19056" xr2:uid="{105007D1-3349-4DE1-98DB-E13B52CA6D09}"/>
   </bookViews>
@@ -918,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5AD71B5-B711-430F-A68D-7C24D0F96FB6}">
   <dimension ref="A1:A172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1018,7 @@
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1093,7 +1093,7 @@
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1123,7 +1123,7 @@
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1153,12 +1153,12 @@
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1173,22 +1173,22 @@
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add initial seaport addons
others haven't been found (et)
</commit_message>
<xml_diff>
--- a/src/yaml/stex-custodian/CDK3 Progress.xlsx
+++ b/src/yaml/stex-custodian/CDK3 Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\repos\simtropolis-channel\src\yaml\stex-custodian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438E5D5F-0476-4653-8B63-4201910ECE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5287C2E-96A0-4E65-8B15-E9A68EFC5805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2376" yWindow="17172" windowWidth="34776" windowHeight="19056" xr2:uid="{105007D1-3349-4DE1-98DB-E13B52CA6D09}"/>
   </bookViews>
@@ -551,7 +551,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -561,6 +561,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,11 +583,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5AD71B5-B711-430F-A68D-7C24D0F96FB6}">
   <dimension ref="A1:A172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,12 +1090,12 @@
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1098,27 +1105,27 @@
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1128,17 +1135,17 @@
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1148,7 +1155,7 @@
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1163,12 +1170,12 @@
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1193,177 +1200,177 @@
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="3" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1378,7 +1385,7 @@
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="3" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1393,7 +1400,7 @@
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="3" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1403,32 +1410,32 @@
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="A97" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="A101" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1468,17 +1475,17 @@
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="A110" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="A111" s="3" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1513,127 +1520,127 @@
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="A118" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+      <c r="A119" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="A120" s="4" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="A121" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+      <c r="A122" s="4" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="A123" s="4" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+      <c r="A124" s="4" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+      <c r="A125" s="4" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+      <c r="A126" s="4" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="A127" s="4" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+      <c r="A128" s="4" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+      <c r="A129" s="4" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+      <c r="A130" s="4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="A131" s="4" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="A132" s="4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+      <c r="A133" s="4" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
+      <c r="A134" s="4" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="A135" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+      <c r="A136" s="4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+      <c r="A137" s="4" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+      <c r="A138" s="4" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
+      <c r="A139" s="4" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
+      <c r="A140" s="4" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
+      <c r="A141" s="4" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
+      <c r="A142" s="4" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1648,12 +1655,12 @@
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
+      <c r="A145" s="4" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
+      <c r="A146" s="4" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1673,7 +1680,7 @@
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
+      <c r="A150" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1688,7 +1695,7 @@
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
+      <c r="A153" s="3" t="s">
         <v>144</v>
       </c>
     </row>

</xml_diff>